<commit_message>
committed on 25 oct 2018
</commit_message>
<xml_diff>
--- a/Decorist_Legacy1/src/main/java/TestData/Decorist_Legacy.xlsx
+++ b/Decorist_Legacy1/src/main/java/TestData/Decorist_Legacy.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65E1CA89-5A4A-42CA-B437-A81114A6B32A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{112C5CE6-95C8-4CBC-84A9-F473D1E0736F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,9 @@
     <sheet name="ShoppingCart" sheetId="6" r:id="rId5"/>
     <sheet name="UI" sheetId="7" r:id="rId6"/>
     <sheet name="Images" sheetId="4" r:id="rId7"/>
+    <sheet name="Designers" sheetId="8" r:id="rId8"/>
+    <sheet name="Email" sheetId="9" r:id="rId9"/>
+    <sheet name="AdminDashboard" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="234">
   <si>
     <t>Client Login</t>
   </si>
@@ -103,9 +106,6 @@
     <t>chair.jpeg</t>
   </si>
   <si>
-    <t>Page Name</t>
-  </si>
-  <si>
     <t>URL</t>
   </si>
   <si>
@@ -154,15 +154,6 @@
     <t>Thanks for ordering</t>
   </si>
   <si>
-    <t>DINING ROOM</t>
-  </si>
-  <si>
-    <t>CLASSIC DESIGN</t>
-  </si>
-  <si>
-    <t>$299</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
@@ -175,18 +166,6 @@
     <t>Design Package</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>$897</t>
-  </si>
-  <si>
-    <t>DEN</t>
-  </si>
-  <si>
-    <t>PLAYROOM</t>
-  </si>
-  <si>
     <t>Room Details</t>
   </si>
   <si>
@@ -199,9 +178,6 @@
     <t>We’ve received your project details,</t>
   </si>
   <si>
-    <t>Your designer won’t be matched until your details are submitted. You can review your answers below to make any final edits.</t>
-  </si>
-  <si>
     <t>Sections Complete</t>
   </si>
   <si>
@@ -224,9 +200,6 @@
   </si>
   <si>
     <t>You’ll be matched by us!</t>
-  </si>
-  <si>
-    <t>Have any designers in mind? Let us know and we’ll check their availability first.</t>
   </si>
   <si>
     <t>Designers &gt;</t>
@@ -355,12 +328,444 @@
   <si>
     <t>not open to new layout</t>
   </si>
+  <si>
+    <t>CELEBRITY DESIGN</t>
+  </si>
+  <si>
+    <t>$1,299</t>
+  </si>
+  <si>
+    <t>ELITE DESIGN</t>
+  </si>
+  <si>
+    <t>$599</t>
+  </si>
+  <si>
+    <t>$1,198</t>
+  </si>
+  <si>
+    <t>$3,096</t>
+  </si>
+  <si>
+    <t>NURSERY</t>
+  </si>
+  <si>
+    <t>OTHER</t>
+  </si>
+  <si>
+    <t>Classic Designers</t>
+  </si>
+  <si>
+    <t>Elite Designers</t>
+  </si>
+  <si>
+    <t>Celebrity Designers</t>
+  </si>
+  <si>
+    <t>Lauren</t>
+  </si>
+  <si>
+    <t>Your designer won’t be matched until 
+your details are submitted. You can review your answers below to make any final edits.</t>
+  </si>
+  <si>
+    <t>Have any designers in mind? Let us know and we’ll 
+check their availability first.</t>
+  </si>
+  <si>
+    <t>Designers</t>
+  </si>
+  <si>
+    <t>MEET OUR DESIGNERS</t>
+  </si>
+  <si>
+    <t>meetOurDesigners</t>
+  </si>
+  <si>
+    <t>Our interior designers are hand-selected across three experience levels ranging from talented newcomers to notable names in the industry.</t>
+  </si>
+  <si>
+    <t>ourInteriorDesigners</t>
+  </si>
+  <si>
+    <t>amountPerRoomClassic</t>
+  </si>
+  <si>
+    <t>amountPerRoomElite</t>
+  </si>
+  <si>
+    <t>amountPerRoomCelebrity</t>
+  </si>
+  <si>
+    <t>299
+per
+room</t>
+  </si>
+  <si>
+    <t>599
+per
+room</t>
+  </si>
+  <si>
+    <t>1,299
+per
+room</t>
+  </si>
+  <si>
+    <t>Our best value. Instagram-worthy style that doesn't equal high price.</t>
+  </si>
+  <si>
+    <t>aboutClassic</t>
+  </si>
+  <si>
+    <t>GREAT FOR:</t>
+  </si>
+  <si>
+    <t>INCLUDES:</t>
+  </si>
+  <si>
+    <t>greatFor</t>
+  </si>
+  <si>
+    <t>includes</t>
+  </si>
+  <si>
+    <t>Design that adapts to your lifestyle</t>
+  </si>
+  <si>
+    <t>Two initial design concepts to review, final room design and floor plan, online shopping list, complimentary purchasing service, direct messaging with your designer</t>
+  </si>
+  <si>
+    <t>greatForClassic</t>
+  </si>
+  <si>
+    <t>includesClassic</t>
+  </si>
+  <si>
+    <t>seasonedTalent</t>
+  </si>
+  <si>
+    <t>Tapping a designer’s signature look</t>
+  </si>
+  <si>
+    <t>tappingADesigner</t>
+  </si>
+  <si>
+    <t>aboutCelebrity</t>
+  </si>
+  <si>
+    <t>Making an investment in your space with celebrity style</t>
+  </si>
+  <si>
+    <t>makingInvestment</t>
+  </si>
+  <si>
+    <t>twoInitialMoodboards</t>
+  </si>
+  <si>
+    <t>Seasoned talent with 5+ years of successful design projects.</t>
+  </si>
+  <si>
+    <t>High-profile designers you’ve eyed on social media and in top magazines.</t>
+  </si>
+  <si>
+    <t>Two initial moodboards to review, one design concept and accessory board, final room design and floor plan, online shopping list, complimentary purchasing service
+PLUS! Personal project manager, direct messaging with project manager, 30 minute call with project manager</t>
+  </si>
+  <si>
+    <t>abc@.com</t>
+  </si>
+  <si>
+    <t>Err Msg</t>
+  </si>
+  <si>
+    <t>Please enter a valid email.</t>
+  </si>
+  <si>
+    <t>Please enter a valid password. Note that passwords are case-sensitive.</t>
+  </si>
+  <si>
+    <t>mishra.sr89@gmail.com</t>
+  </si>
+  <si>
+    <t>shubhanshum22</t>
+  </si>
+  <si>
+    <t>abcvv</t>
+  </si>
+  <si>
+    <t>Please enter a valid email and password. Note that passwords are case-sensitive.</t>
+  </si>
+  <si>
+    <t>shubhanshu.mishra@intsof.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                        New user signup</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Akash</t>
+  </si>
+  <si>
+    <t>singhal</t>
+  </si>
+  <si>
+    <t>HostName</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>From</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>outlook.office365.com</t>
+  </si>
+  <si>
+    <t>Decorist &lt;yourteam@decorist.com&gt;</t>
+  </si>
+  <si>
+    <t>Thanks for Your Decorist Room Design Purchase!</t>
+  </si>
+  <si>
+    <t>Welcome to Decorist, Your Online Personal Home Designer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                 Admin Login</t>
+  </si>
+  <si>
+    <t>Password12</t>
+  </si>
+  <si>
+    <t>anmol.aggarwal+admin@decorist.com</t>
+  </si>
+  <si>
+    <t>https://www.idcqa.decorist.com/admin/orders/promocodediscount/</t>
+  </si>
+  <si>
+    <t>Client Page Name</t>
+  </si>
+  <si>
+    <t>Admin Page Name</t>
+  </si>
+  <si>
+    <t>Home Page</t>
+  </si>
+  <si>
+    <t>https://www.idcqa.decorist.com/admin/</t>
+  </si>
+  <si>
+    <t>Promo Codes</t>
+  </si>
+  <si>
+    <t>receivedProDetails</t>
+  </si>
+  <si>
+    <t>anmol aggarwal</t>
+  </si>
+  <si>
+    <t>AdminDesignSolutions</t>
+  </si>
+  <si>
+    <t>Strings</t>
+  </si>
+  <si>
+    <t>attentionStr</t>
+  </si>
+  <si>
+    <t>!Attention!</t>
+  </si>
+  <si>
+    <t>To Assign a designer to solutions select a designer from list.</t>
+  </si>
+  <si>
+    <t>toAssignDesignerStr</t>
+  </si>
+  <si>
+    <t>To Un-assign designer from solutions don't select any designer.</t>
+  </si>
+  <si>
+    <t>toUnAssignDesignerStr</t>
+  </si>
+  <si>
+    <t>Successfully assigned designer</t>
+  </si>
+  <si>
+    <t>successfulAssignDesigner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               Designer Login</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>anmol.aggarwal+designer@decorist.com</t>
+  </si>
+  <si>
+    <t>Style quiz page</t>
+  </si>
+  <si>
+    <t>https://www.idcqa.decorist.com/lp/style-quiz/</t>
+  </si>
+  <si>
+    <t>you are [modern]</t>
+  </si>
+  <si>
+    <t>https://www.dev.decorist.com/questionnaire/result/</t>
+  </si>
+  <si>
+    <t>Order Total</t>
+  </si>
+  <si>
+    <t>designPackageForNonLogin</t>
+  </si>
+  <si>
+    <t>https://www.dev.decorist.com/order/select-level/</t>
+  </si>
+  <si>
+    <t>Shopping Cart pageNonLogin</t>
+  </si>
+  <si>
+    <t>https://www.dev.decorist.com/order/checkout/</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>HOME OFFICE</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Items Details Page</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>Now, let’s talk furniture.</t>
+  </si>
+  <si>
+    <t>Do you want to keep any of your existing furniture?</t>
+  </si>
+  <si>
+    <t>List only the main items you’ll be keeping.</t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>Dimensions</t>
+  </si>
+  <si>
+    <t>Feet</t>
+  </si>
+  <si>
+    <t>Retailer</t>
+  </si>
+  <si>
+    <t>Optional</t>
+  </si>
+  <si>
+    <t>What items do you want to replace?</t>
+  </si>
+  <si>
+    <t>What items do you want to add?</t>
+  </si>
+  <si>
+    <t>Let your designer know if you have any detailed item needs.</t>
+  </si>
+  <si>
+    <t>Want to avoid materials that show pet dander? Allergic to feathers?</t>
+  </si>
+  <si>
+    <t>Are you open to painting your room?</t>
+  </si>
+  <si>
+    <t>Are you open to wallpaper?</t>
+  </si>
+  <si>
+    <t>Are you open to drapes or window treatments?</t>
+  </si>
+  <si>
+    <t>Inspiration Page</t>
+  </si>
+  <si>
+    <t>Let’s see what style you’d like for your home office.</t>
+  </si>
+  <si>
+    <t>Select at least 3 photos that best reflect the look and feel you want.</t>
+  </si>
+  <si>
+    <t>What do you like about this photo? Is there anything you dislike?</t>
+  </si>
+  <si>
+    <t>Is it the overall look and feel? Colors or patterns? A specific furniture item?</t>
+  </si>
+  <si>
+    <t>You like a mostly</t>
+  </si>
+  <si>
+    <t>Refine this further for your designer by adding your own links or photos below.</t>
+  </si>
+  <si>
+    <t>ADD LINKS</t>
+  </si>
+  <si>
+    <t>Add links to the items you love or any Pinterest boards or Houzz pages you’ve been working on. Simply copy and paste the full links below (and make sure your Pinterest boards aren’t private!)</t>
+  </si>
+  <si>
+    <t>ADD PHOTOS</t>
+  </si>
+  <si>
+    <t>Comments on photos are required.</t>
+  </si>
+  <si>
+    <t>Upload room photos or other design inspiration below and add comments. If you don’t have any saved, take a look at our Pinterest board for inspiration!</t>
+  </si>
+  <si>
+    <t>You’re almost done!</t>
+  </si>
+  <si>
+    <t>What’s your overall color preference?</t>
+  </si>
+  <si>
+    <t>What’s your budget for furniture, accessories, paint, etc?</t>
+  </si>
+  <si>
+    <t>This helps your designer recommend the best items curated just for you. This budget will not include tax, shipping, or installation costs.</t>
+  </si>
+  <si>
+    <t>ImageSRC</t>
+  </si>
+  <si>
+    <t>Neutral palette</t>
+  </si>
+  <si>
+    <t>Do you have a specific budget in mind?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -401,8 +806,31 @@
       <color rgb="FF333333"/>
       <name val="ProximaNova-Reg"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF666666"/>
+      <name val="ProximaNova-Reg"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF666666"/>
+      <name val="ProximaNova-Reg"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="ProximaNova-Bold"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -439,6 +867,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -453,7 +893,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -463,6 +903,22 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -473,7 +929,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -755,34 +1214,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:Q8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="30.42578125" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="11.42578125" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="11.7109375" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="28.7109375" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="11.5703125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="84.7109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="24.42578125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18.7109375" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="32.5703125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="44.42578125" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="31.140625" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="37.7109375" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="16.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:17">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="11" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-    </row>
-    <row r="2" spans="1:6" s="2" customFormat="1">
+      <c r="D1" s="21"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="M1" s="24"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+    </row>
+    <row r="2" spans="1:17" s="2" customFormat="1">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -801,8 +1286,38 @@
       <c r="F2" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -821,20 +1336,167 @@
       <c r="F3" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="G3" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="H3" t="s">
+        <v>151</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="M3" t="s">
+        <v>162</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="P3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" t="s">
+        <v>142</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="5">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:F1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="O1:Q1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1" xr:uid="{B7BF400E-FB10-4EBF-BB26-8D7644E899CA}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{598D5F9A-07D7-4B51-9EF2-416E5E9986C9}"/>
     <hyperlink ref="E3" r:id="rId3" xr:uid="{C8B4834F-7D33-48F4-8199-99EB6658F176}"/>
     <hyperlink ref="F3" r:id="rId4" xr:uid="{0A9D2BFC-88A0-4CD8-AE72-35C989C59253}"/>
+    <hyperlink ref="E4" r:id="rId5" xr:uid="{AAB3FF47-0AC7-4950-A462-F6FD83C7BA13}"/>
+    <hyperlink ref="F4" r:id="rId6" xr:uid="{BFA3B420-04D9-4A17-9BC7-409A561539FA}"/>
+    <hyperlink ref="E5" r:id="rId7" xr:uid="{DFD72DC4-CB2F-4073-A3EF-2A21BF344C36}"/>
+    <hyperlink ref="E6" r:id="rId8" xr:uid="{BAA02EA2-D34C-4915-B9DC-529517DB4E3A}"/>
+    <hyperlink ref="F6" r:id="rId9" xr:uid="{0E11B1AA-A314-45CF-AB71-7A0CA652B51D}"/>
+    <hyperlink ref="B7" r:id="rId10" xr:uid="{B73DF86C-6EF3-4E9B-8BBB-2B8FA87F4FED}"/>
+    <hyperlink ref="A4" r:id="rId11" display="shubhanshum22@gmail.com" xr:uid="{38EAE7E1-0615-487F-89B6-809C898596A5}"/>
+    <hyperlink ref="B4" r:id="rId12" xr:uid="{24BC8EB0-D925-44EF-8B1E-C32C83ACDD0C}"/>
+    <hyperlink ref="A5" r:id="rId13" xr:uid="{067BA417-4ED2-41DF-9CD8-DCAB51E26558}"/>
+    <hyperlink ref="A6" r:id="rId14" xr:uid="{1864B0C4-3EF9-454B-BC4E-C2EC0951A404}"/>
+    <hyperlink ref="A8" r:id="rId15" xr:uid="{B99983F3-F1DA-4341-95AD-AA171C8C4AB0}"/>
+    <hyperlink ref="B8" r:id="rId16" xr:uid="{C88DA719-13F9-4CFF-83B2-DAA656194E15}"/>
+    <hyperlink ref="K3" r:id="rId17" xr:uid="{836E4146-4A6E-4A3B-B198-5BB8F13ED0E1}"/>
+    <hyperlink ref="L3" r:id="rId18" xr:uid="{BEBC8F97-60DF-4971-90F8-1D58F3B6A200}"/>
+    <hyperlink ref="L4" r:id="rId19" xr:uid="{6FC58AE9-93E6-407E-ABAB-D36B26A03E1A}"/>
+    <hyperlink ref="O3" r:id="rId20" xr:uid="{12A5447D-7528-47AC-A212-673C4DA12D5C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId21"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09952573-2FCC-4492-8549-085CEC287EB0}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="36.42578125" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="18" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -842,7 +1504,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F45ED6A-4059-4CBD-B0EE-319F51313DF2}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -862,13 +1526,10 @@
       <c r="A2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="3" spans="1:2">
       <c r="B3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -879,69 +1540,134 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CF382EA-42BF-40B2-98B4-D29AF291B646}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="90.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="66.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="4" customFormat="1">
+    <row r="1" spans="1:6" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>27</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>29</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>31</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>33</v>
       </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>35</v>
       </c>
-      <c r="B6" t="s">
-        <v>36</v>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>186</v>
+      </c>
+      <c r="B7" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>188</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>191</v>
+      </c>
+      <c r="B9" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>193</v>
+      </c>
+      <c r="B10" t="s">
+        <v>194</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B8" r:id="rId1" xr:uid="{36473CC7-9DD7-4726-BFE9-4E720D3BD7D6}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -963,21 +1689,21 @@
   <sheetData>
     <row r="1" spans="1:4" s="5" customFormat="1">
       <c r="A1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B2">
         <v>1123</v>
@@ -999,111 +1725,118 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9FB3A7D-8435-4B0E-BF9B-F42CA196F52D}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="17.140625" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="20.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.85546875" customWidth="1"/>
+    <col min="10" max="10" width="39.28515625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1">
-      <c r="B1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>92</v>
+    <row r="1" spans="1:11" s="17" customFormat="1">
+      <c r="B1" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>195</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>196</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>95</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>96</v>
       </c>
       <c r="E2" t="s">
-        <v>45</v>
+        <v>197</v>
       </c>
       <c r="F2" t="s">
-        <v>44</v>
+        <v>97</v>
       </c>
       <c r="G2" t="s">
-        <v>50</v>
+        <v>98</v>
       </c>
       <c r="H2" t="s">
-        <v>50</v>
+        <v>98</v>
+      </c>
+      <c r="I2" t="s">
+        <v>98</v>
       </c>
       <c r="K2" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="B3" t="s">
-        <v>51</v>
+        <v>99</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>95</v>
       </c>
       <c r="D3" t="s">
-        <v>44</v>
+        <v>96</v>
       </c>
       <c r="E3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F3" t="s">
-        <v>44</v>
+        <v>97</v>
       </c>
       <c r="G3" t="s">
-        <v>50</v>
+        <v>98</v>
       </c>
       <c r="K3" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="B4" t="s">
-        <v>52</v>
+        <v>100</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>93</v>
       </c>
       <c r="D4" t="s">
-        <v>44</v>
+        <v>94</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F4" t="s">
-        <v>44</v>
+        <v>97</v>
       </c>
       <c r="G4" t="s">
-        <v>50</v>
+        <v>98</v>
       </c>
       <c r="K4" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="K5" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="K6" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1114,203 +1847,450 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5586D3A0-1D2B-4AE1-8ABC-14A7A7C3FEBD}">
-  <dimension ref="C1:L20"/>
+  <dimension ref="C1:P20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E7" workbookViewId="0">
+    <sheetView topLeftCell="J13" workbookViewId="0">
       <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="4" max="4" width="74.7109375" customWidth="1"/>
-    <col min="9" max="9" width="20.5703125" customWidth="1"/>
-    <col min="11" max="11" width="16.28515625" customWidth="1"/>
-    <col min="12" max="12" width="37.42578125" customWidth="1"/>
+    <col min="3" max="3" width="30" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="74.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="30.85546875" customWidth="1"/>
+    <col min="7" max="7" width="21" customWidth="1"/>
+    <col min="8" max="8" width="69.28515625" customWidth="1"/>
+    <col min="9" max="9" width="20.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="36.140625" customWidth="1"/>
+    <col min="11" max="11" width="23.28515625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="51.5703125" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="24.85546875" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="60.28515625" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="23.28515625" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="28.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:12" s="8" customFormat="1">
+    <row r="1" spans="3:16" s="8" customFormat="1">
       <c r="C1" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="P1" s="8" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="3:16">
+      <c r="C2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" t="s">
         <v>53</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="F2" t="s">
+        <v>200</v>
+      </c>
+      <c r="H2" t="s">
+        <v>216</v>
+      </c>
+      <c r="J2" t="s">
+        <v>227</v>
+      </c>
+      <c r="K2" t="s">
+        <v>60</v>
+      </c>
+      <c r="L2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M2" t="s">
+        <v>109</v>
+      </c>
+      <c r="N2" t="s">
+        <v>108</v>
+      </c>
+      <c r="O2" t="s">
+        <v>174</v>
+      </c>
+      <c r="P2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="3" spans="3:16">
+      <c r="C3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" t="s">
+        <v>201</v>
+      </c>
+      <c r="H3" t="s">
+        <v>217</v>
+      </c>
+      <c r="J3" t="s">
+        <v>228</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M3" t="s">
+        <v>111</v>
+      </c>
+      <c r="N3" t="s">
+        <v>110</v>
+      </c>
+      <c r="O3" t="s">
+        <v>177</v>
+      </c>
+      <c r="P3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="4" spans="3:16" ht="45">
+      <c r="C4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4" t="s">
+        <v>202</v>
+      </c>
+      <c r="H4" t="s">
+        <v>218</v>
+      </c>
+      <c r="J4" t="s">
+        <v>229</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="M4" t="s">
+        <v>112</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="O4" t="s">
+        <v>179</v>
+      </c>
+      <c r="P4" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="5" spans="3:16" ht="45">
+      <c r="C5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="H5" t="s">
+        <v>219</v>
+      </c>
+      <c r="J5" t="s">
+        <v>230</v>
+      </c>
+      <c r="K5" t="s">
+        <v>170</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="M5" t="s">
+        <v>113</v>
+      </c>
+      <c r="N5" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="O5" t="s">
+        <v>181</v>
+      </c>
+      <c r="P5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="6" spans="3:16" ht="45">
+      <c r="C6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F6" t="s">
+        <v>203</v>
+      </c>
+      <c r="H6" t="s">
+        <v>220</v>
+      </c>
+      <c r="J6" t="s">
+        <v>233</v>
+      </c>
+      <c r="L6" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="M6" t="s">
+        <v>114</v>
+      </c>
+      <c r="N6" s="10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="3:16" ht="30">
+      <c r="C7" t="s">
         <v>71</v>
       </c>
-      <c r="K1" s="8" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="3:12">
-      <c r="C2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D2" t="s">
-        <v>62</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="D7" t="s">
         <v>70</v>
       </c>
-      <c r="L2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="3:12">
-      <c r="C3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D3" t="s">
-        <v>73</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="3:12">
-      <c r="C4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D4" t="s">
-        <v>75</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="3:12">
-      <c r="C5" t="s">
-        <v>78</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="3:12">
-      <c r="C6" t="s">
-        <v>82</v>
-      </c>
-      <c r="D6" t="s">
-        <v>79</v>
-      </c>
-      <c r="L6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="3:12">
-      <c r="C7" t="s">
-        <v>81</v>
-      </c>
-      <c r="D7" t="s">
-        <v>80</v>
+      <c r="F7" t="s">
+        <v>204</v>
+      </c>
+      <c r="H7" t="s">
+        <v>221</v>
       </c>
       <c r="L7" s="7">
         <v>43194</v>
       </c>
-    </row>
-    <row r="8" spans="3:12">
+      <c r="M7" t="s">
+        <v>119</v>
+      </c>
+      <c r="N7" s="10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="3:16">
       <c r="C8" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>83</v>
+        <v>73</v>
+      </c>
+      <c r="F8" t="s">
+        <v>205</v>
+      </c>
+      <c r="H8" t="s">
+        <v>222</v>
       </c>
       <c r="L8" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="M8" t="s">
+        <v>122</v>
+      </c>
+      <c r="N8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="3:16">
+      <c r="C9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9" t="s">
+        <v>206</v>
+      </c>
+      <c r="H9" t="s">
+        <v>223</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="M9" t="s">
+        <v>123</v>
+      </c>
+      <c r="N9" s="10" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="3:16">
+      <c r="C10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D10" t="s">
+        <v>76</v>
+      </c>
+      <c r="F10" t="s">
+        <v>207</v>
+      </c>
+      <c r="H10" t="s">
+        <v>226</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="M10" t="s">
+        <v>126</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="3:16" ht="45">
+      <c r="C11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" t="s">
+        <v>79</v>
+      </c>
+      <c r="F11" t="s">
+        <v>208</v>
+      </c>
+      <c r="H11" t="s">
+        <v>224</v>
+      </c>
+      <c r="K11" t="s">
+        <v>52</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="M11" t="s">
+        <v>127</v>
+      </c>
+      <c r="N11" s="10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="3:16">
+      <c r="C12" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="F12" t="s">
+        <v>209</v>
+      </c>
+      <c r="H12" t="s">
+        <v>225</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="M12" t="s">
+        <v>128</v>
+      </c>
+      <c r="N12" s="10" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="13" spans="3:16">
+      <c r="F13" t="s">
+        <v>210</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="M13" t="s">
+        <v>130</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="14" spans="3:16" ht="30">
+      <c r="F14" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="M14" t="s">
+        <v>131</v>
+      </c>
+      <c r="N14" s="10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="15" spans="3:16">
+      <c r="F15" t="s">
+        <v>212</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="M15" t="s">
+        <v>133</v>
+      </c>
+      <c r="N15" s="11" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="3:16" ht="72">
+      <c r="F16" t="s">
+        <v>213</v>
+      </c>
+      <c r="L16" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="M16" t="s">
+        <v>134</v>
+      </c>
+      <c r="N16" s="13" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="17" spans="6:14">
+      <c r="F17" t="s">
+        <v>214</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="N17" s="12"/>
+    </row>
+    <row r="18" spans="6:14">
+      <c r="L18" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="3:12">
-      <c r="C9" t="s">
-        <v>85</v>
-      </c>
-      <c r="D9" t="s">
-        <v>85</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="3:12">
-      <c r="C10" t="s">
-        <v>87</v>
-      </c>
-      <c r="D10" t="s">
-        <v>86</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="3:12">
-      <c r="C11" t="s">
-        <v>88</v>
-      </c>
-      <c r="D11" t="s">
+    <row r="19" spans="6:14">
+      <c r="K19" t="s">
+        <v>91</v>
+      </c>
+      <c r="L19" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="K11" t="s">
-        <v>61</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" spans="3:12">
-      <c r="C12" t="s">
+    </row>
+    <row r="20" spans="6:14">
+      <c r="K20" t="s">
+        <v>92</v>
+      </c>
+      <c r="L20" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="L12" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="3:12">
-      <c r="L13" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="3:12">
-      <c r="L14" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="3:12">
-      <c r="L15" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16" spans="3:12">
-      <c r="L16" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="11:12">
-      <c r="L17" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="11:12">
-      <c r="L18" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" spans="11:12">
-      <c r="K19" t="s">
-        <v>101</v>
-      </c>
-      <c r="L19" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="20" spans="11:12">
-      <c r="K20" t="s">
-        <v>102</v>
-      </c>
-      <c r="L20" s="3" t="s">
-        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1386,4 +2366,102 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE1E62FA-702C-40A9-8477-D2D8C9E348CD}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.140625" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="4" customFormat="1">
+      <c r="A1" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="B2" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D82F4FB-4DC8-45A9-920B-31BE3CD6550E}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="21.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="29.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="34.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="52.42578125" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="5" customFormat="1">
+      <c r="A1" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="E3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
commited on oct 26,2018
</commit_message>
<xml_diff>
--- a/Decorist_Legacy1/src/main/java/TestData/Decorist_Legacy.xlsx
+++ b/Decorist_Legacy1/src/main/java/TestData/Decorist_Legacy.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{112C5CE6-95C8-4CBC-84A9-F473D1E0736F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07742FCF-8ED0-44F3-9324-EE5884315CEA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="236">
   <si>
     <t>Client Login</t>
   </si>
@@ -644,15 +644,6 @@
     <t>https://www.dev.decorist.com/order/checkout/</t>
   </si>
   <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>HOME OFFICE</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>Items Details Page</t>
   </si>
   <si>
@@ -759,12 +750,28 @@
   </si>
   <si>
     <t>Do you have a specific budget in mind?</t>
+  </si>
+  <si>
+    <t>singh</t>
+  </si>
+  <si>
+    <t>digvj</t>
+  </si>
+  <si>
+    <t>digvj@gmail.com</t>
+  </si>
+  <si>
+    <t>DINING ROOM</t>
+  </si>
+  <si>
+    <t>bca@1234</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="10">
     <font>
       <sz val="11"/>
@@ -919,6 +926,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -932,7 +940,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1217,55 +1224,55 @@
   <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="28.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="84.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="24.42578125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="18.7109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="32.5703125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="44.42578125" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="31.140625" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="37.7109375" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="16.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="30.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="28.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="84.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="24.42578125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="32.5703125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="44.42578125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="31.140625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="37.7109375" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="16.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="21" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="21"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
       <c r="G1" s="14"/>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="24" t="s">
         <v>147</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
       <c r="K1" s="14"/>
-      <c r="L1" s="24" t="s">
+      <c r="L1" s="25" t="s">
         <v>161</v>
       </c>
-      <c r="M1" s="24"/>
+      <c r="M1" s="25"/>
       <c r="N1" s="16"/>
-      <c r="O1" s="25" t="s">
+      <c r="O1" s="26" t="s">
         <v>182</v>
       </c>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
     </row>
     <row r="2" spans="1:17" s="2" customFormat="1">
       <c r="A2" s="2" t="s">
@@ -1436,6 +1443,18 @@
         <v>142</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>232</v>
+      </c>
+      <c r="D7" t="s">
+        <v>231</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1476,9 +1495,11 @@
     <hyperlink ref="L3" r:id="rId18" xr:uid="{BEBC8F97-60DF-4971-90F8-1D58F3B6A200}"/>
     <hyperlink ref="L4" r:id="rId19" xr:uid="{6FC58AE9-93E6-407E-ABAB-D36B26A03E1A}"/>
     <hyperlink ref="O3" r:id="rId20" xr:uid="{12A5447D-7528-47AC-A212-673C4DA12D5C}"/>
+    <hyperlink ref="E7" r:id="rId21" xr:uid="{9C80B3BC-3B8E-4A65-8FC9-82CD080B65E3}"/>
+    <hyperlink ref="F7" r:id="rId22" xr:uid="{C7B4A8E7-DA77-480C-9BDB-B44C2A6DF865}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId21"/>
+  <pageSetup orientation="portrait" r:id="rId23"/>
 </worksheet>
 </file>
 
@@ -1490,7 +1511,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="36.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" s="18" customFormat="1"/>
@@ -1510,8 +1531,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="102.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="27.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="102.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="2" customFormat="1">
@@ -1548,11 +1569,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="90.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="66.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="34.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="90.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="66.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="26.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="4" customFormat="1">
@@ -1569,7 +1590,7 @@
         <v>25</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>25</v>
@@ -1588,8 +1609,8 @@
       <c r="D2" t="s">
         <v>168</v>
       </c>
-      <c r="E2" s="26" t="s">
-        <v>232</v>
+      <c r="E2" s="19" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1681,10 +1702,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="5" customFormat="1">
@@ -1731,10 +1752,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="17.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.28515625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="39.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="17.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="39.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="16.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="17" customFormat="1">
@@ -1753,28 +1774,28 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="B2" t="s">
-        <v>196</v>
+        <v>234</v>
       </c>
       <c r="C2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E2" t="s">
-        <v>197</v>
+        <v>41</v>
       </c>
       <c r="F2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="I2" t="s">
         <v>98</v>
@@ -1855,20 +1876,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="30" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="74.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
-    <col min="6" max="6" width="30.85546875" customWidth="1"/>
-    <col min="7" max="7" width="21" customWidth="1"/>
-    <col min="8" max="8" width="69.28515625" customWidth="1"/>
-    <col min="9" max="9" width="20.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="36.140625" customWidth="1"/>
-    <col min="11" max="11" width="23.28515625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="51.5703125" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="24.85546875" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="60.28515625" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="23.28515625" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="28.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="30.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="74.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="30.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="69.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="20.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="36.140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="51.5703125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="60.28515625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="28.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="3:16" s="8" customFormat="1">
@@ -1876,22 +1897,22 @@
         <v>45</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="I1" s="8" t="s">
         <v>61</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="K1" s="8" t="s">
         <v>88</v>
@@ -1917,13 +1938,13 @@
         <v>53</v>
       </c>
       <c r="F2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="H2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="J2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="K2" t="s">
         <v>60</v>
@@ -1952,13 +1973,13 @@
         <v>63</v>
       </c>
       <c r="F3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="H3" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="J3" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>46</v>
@@ -1984,13 +2005,13 @@
         <v>65</v>
       </c>
       <c r="F4" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H4" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="J4" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="L4" s="3" t="s">
         <v>47</v>
@@ -2016,10 +2037,10 @@
         <v>67</v>
       </c>
       <c r="H5" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="J5" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="K5" t="s">
         <v>170</v>
@@ -2048,13 +2069,13 @@
         <v>69</v>
       </c>
       <c r="F6" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="H6" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="J6" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="L6" s="10" t="s">
         <v>105</v>
@@ -2074,10 +2095,10 @@
         <v>70</v>
       </c>
       <c r="F7" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="H7" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="L7" s="7">
         <v>43194</v>
@@ -2097,10 +2118,10 @@
         <v>73</v>
       </c>
       <c r="F8" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="H8" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="L8" s="3" t="s">
         <v>49</v>
@@ -2120,10 +2141,10 @@
         <v>75</v>
       </c>
       <c r="F9" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="H9" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="L9" s="3" t="s">
         <v>50</v>
@@ -2143,10 +2164,10 @@
         <v>76</v>
       </c>
       <c r="F10" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="H10" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="L10" s="3" t="s">
         <v>51</v>
@@ -2166,10 +2187,10 @@
         <v>79</v>
       </c>
       <c r="F11" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="H11" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="K11" t="s">
         <v>52</v>
@@ -2192,10 +2213,10 @@
         <v>81</v>
       </c>
       <c r="F12" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="H12" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="L12" s="3" t="s">
         <v>53</v>
@@ -2209,7 +2230,7 @@
     </row>
     <row r="13" spans="3:16">
       <c r="F13" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="L13" s="3" t="s">
         <v>54</v>
@@ -2223,7 +2244,7 @@
     </row>
     <row r="14" spans="3:16" ht="30">
       <c r="F14" s="3" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="L14" s="3" t="s">
         <v>55</v>
@@ -2237,7 +2258,7 @@
     </row>
     <row r="15" spans="3:16">
       <c r="F15" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L15" s="3" t="s">
         <v>56</v>
@@ -2251,7 +2272,7 @@
     </row>
     <row r="16" spans="3:16" ht="72">
       <c r="F16" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="L16" s="10" t="s">
         <v>106</v>
@@ -2265,7 +2286,7 @@
     </row>
     <row r="17" spans="6:14">
       <c r="F17" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="L17" s="3" t="s">
         <v>57</v>
@@ -2309,7 +2330,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="16.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" s="2" customFormat="1">
@@ -2372,15 +2393,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE1E62FA-702C-40A9-8477-D2D8C9E348CD}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="22.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="24.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1">
@@ -2412,16 +2433,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D82F4FB-4DC8-45A9-920B-31BE3CD6550E}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="34.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="52.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="34.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="52.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="5" customFormat="1">
@@ -2448,6 +2469,9 @@
       <c r="B2" t="s">
         <v>146</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>235</v>
+      </c>
       <c r="D2" t="s">
         <v>158</v>
       </c>
@@ -2461,7 +2485,10 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{5126513F-BB27-4717-A64D-D0886BD7E8E1}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>